<commit_message>
Sector AVG working now
</commit_message>
<xml_diff>
--- a/excel_data/input_user.xlsx
+++ b/excel_data/input_user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midaspavia/Documents/python_projects/excel_data_script/excel_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ADF6E9-50CC-1D40-B417-EA213874B5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07C0E3C-3112-F243-92C3-B015ACCC0076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19860" yWindow="-28140" windowWidth="34160" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17780" yWindow="-28140" windowWidth="34160" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>Hermes</t>
-  </si>
-  <si>
     <t>TR.EBIT(Period=FY-1)</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>TR.EBIT(Period=FY-2)</t>
+  </si>
+  <si>
+    <t>BIIB.O</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,17 +471,17 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -489,12 +489,12 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -504,5 +504,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>